<commit_message>
Exercises 1, 2 and 3 done.
</commit_message>
<xml_diff>
--- a/assets/pl_03/2020-03-25-AIBI-PL_Leandro_Gabriel.xlsx
+++ b/assets/pl_03/2020-03-25-AIBI-PL_Leandro_Gabriel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud\Onedrive\Pessoal\Acadêmico\FEUP\2019-2020-2-AIBI\PL\assets\pl_03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BFC222A-2102-4145-982B-3825DB58B5F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C470F97E-20EA-4D6E-AA88-0D37A5F14D4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{91FBA814-AE36-401C-A442-96DDE22A50B5}"/>
   </bookViews>
@@ -559,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9CE67C4-97F7-40B1-8303-C645B93F8892}">
   <dimension ref="B1:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.42578125" defaultRowHeight="19.7" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -599,13 +599,13 @@
         <v>1</v>
       </c>
       <c r="O2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:21" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
@@ -631,13 +631,13 @@
         <v>3</v>
       </c>
       <c r="O3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:21" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
@@ -663,13 +663,13 @@
         <v>7</v>
       </c>
       <c r="O4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:21" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>